<commit_message>
close #262: Adds a check when there are 2 or more spaces in a row in the text
</commit_message>
<xml_diff>
--- a/input_data/data_errors_01/descricao.xlsx
+++ b/input_data/data_errors_01/descricao.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Impactos para Segurança Alimentar</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;h1&gt;Consequências esperadas e resultantes das mudanças climáticas em sistemas  &lt;/h1&gt; socioecológicos relacionados à segurança alimentar.</t>
+    <t xml:space="preserve">&lt;h1&gt;Consequências esperadas e resultantes das mudanças climáticas em sistemas &lt;/h1&gt; socioecológicos relacionados à segurança alimentar.</t>
   </si>
   <si>
     <t xml:space="preserve">São os efeitos sobre vidas, meioz de subsistência, saúde, ecossistemas, economias, çociedades, culturas, serviços e infraestrutura, devido a alterações climáticas ou eventos climáticos que se dão dentro de períodos específicos de tempo, de vulnerabilidade e de exposição da sociedade ou sistema, relacionados à segurança alimentar.&lt;br&gt;A Segurança Alimentar e Nutricional (SAN) consiste na realização do direito de todos ao acesso regular e permanente a alimentos de qualidade, em quantidade suficiente, sem comprometer o acesso a outras necessidades essenciais, tendo como base práticas alimentares promotoras de saúde, que respeitem a diversidade cultural e que sejam ambiental, cultural, econômica e socialmente sustentáveis.&lt;br&gt;&lt;br&gt;Fontes:&lt;br&gt;&lt;a href="http://www.planalto.gov.br/ccivil_03/_ato2004-2006/2006/lei/l11346.htm"&gt;BRASIL. LEI Nº 11.346, DE 15 DE SETEMBRO DE 2006. Brasília: 2006.&lt;/a&gt;&lt;br&gt;INTERGOVERNMENTAL PANEL ON CLIMATE CHANGE - IPCC. Climate Change 2014: Synthesis Report. Working Groups I, II and III to the Fifth Assessment Report of the Intergovernmental Panel on Climate Change [Core Writing Team, R.K. Pachauri and L.A. Meyer (eds.)]. IPCC, Geneva, Switzerland, 151 pp</t>
@@ -582,10 +582,10 @@
   </sheetPr>
   <dimension ref="A1:Y866"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>